<commit_message>
Rewrote for season adaptability
</commit_message>
<xml_diff>
--- a/processed_data/2023pncmp.xlsx
+++ b/processed_data/2023pncmp.xlsx
@@ -1239,7 +1239,7 @@
         </is>
       </c>
       <c r="E8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -1663,7 +1663,7 @@
         </is>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1771,7 +1771,7 @@
         </is>
       </c>
       <c r="E13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1983,7 +1983,7 @@
         </is>
       </c>
       <c r="E15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -2091,7 +2091,7 @@
         </is>
       </c>
       <c r="E16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -2831,7 +2831,7 @@
         </is>
       </c>
       <c r="E23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -3147,7 +3147,7 @@
         </is>
       </c>
       <c r="E26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -3255,7 +3255,7 @@
         </is>
       </c>
       <c r="E27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -3467,7 +3467,7 @@
         </is>
       </c>
       <c r="E29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -3575,7 +3575,7 @@
         </is>
       </c>
       <c r="E30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -3899,7 +3899,7 @@
         </is>
       </c>
       <c r="E33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -4223,7 +4223,7 @@
         </is>
       </c>
       <c r="E36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -5519,7 +5519,7 @@
         </is>
       </c>
       <c r="E48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -11425,7 +11425,7 @@
         </is>
       </c>
       <c r="E104" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
@@ -12381,7 +12381,7 @@
         </is>
       </c>
       <c r="E113" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -13209,7 +13209,7 @@
         </is>
       </c>
       <c r="E121" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -14045,7 +14045,7 @@
         </is>
       </c>
       <c r="E129" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F129" t="inlineStr">
         <is>
@@ -14565,7 +14565,7 @@
         </is>
       </c>
       <c r="E134" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
@@ -14773,7 +14773,7 @@
         </is>
       </c>
       <c r="E136" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F136" t="inlineStr">
         <is>
@@ -14882,7 +14882,7 @@
         </is>
       </c>
       <c r="E137" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
@@ -15094,7 +15094,7 @@
         </is>
       </c>
       <c r="E139" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
@@ -15410,7 +15410,7 @@
         </is>
       </c>
       <c r="E142" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F142" t="inlineStr">
         <is>
@@ -16786,7 +16786,7 @@
         </is>
       </c>
       <c r="E155" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F155" t="inlineStr">
         <is>
@@ -17002,7 +17002,7 @@
         </is>
       </c>
       <c r="E157" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F157" t="inlineStr">
         <is>
@@ -18894,7 +18894,7 @@
         </is>
       </c>
       <c r="E175" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F175" t="inlineStr">
         <is>
@@ -19206,7 +19206,7 @@
         </is>
       </c>
       <c r="E178" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F178" t="inlineStr">
         <is>
@@ -19522,7 +19522,7 @@
         </is>
       </c>
       <c r="E181" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F181" t="inlineStr">
         <is>
@@ -20366,7 +20366,7 @@
         </is>
       </c>
       <c r="E189" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F189" t="inlineStr">
         <is>
@@ -20682,7 +20682,7 @@
         </is>
       </c>
       <c r="E192" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F192" t="inlineStr">
         <is>
@@ -20898,7 +20898,7 @@
         </is>
       </c>
       <c r="E194" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F194" t="inlineStr">
         <is>
@@ -22074,7 +22074,7 @@
         </is>
       </c>
       <c r="E205" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F205" t="inlineStr">
         <is>
@@ -24909,7 +24909,7 @@
         </is>
       </c>
       <c r="E232" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F232" t="inlineStr">
         <is>
@@ -25117,7 +25117,7 @@
         </is>
       </c>
       <c r="E234" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F234" t="inlineStr">
         <is>
@@ -25221,7 +25221,7 @@
         </is>
       </c>
       <c r="E235" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F235" t="inlineStr">
         <is>
@@ -25429,7 +25429,7 @@
         </is>
       </c>
       <c r="E237" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F237" t="inlineStr">
         <is>
@@ -25533,7 +25533,7 @@
         </is>
       </c>
       <c r="E238" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F238" t="inlineStr">
         <is>
@@ -25637,7 +25637,7 @@
         </is>
       </c>
       <c r="E239" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F239" t="inlineStr">
         <is>
@@ -25845,7 +25845,7 @@
         </is>
       </c>
       <c r="E241" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F241" t="inlineStr">
         <is>
@@ -25949,7 +25949,7 @@
         </is>
       </c>
       <c r="E242" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F242" t="inlineStr">
         <is>
@@ -26053,7 +26053,7 @@
         </is>
       </c>
       <c r="E243" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F243" t="inlineStr">
         <is>
@@ -26157,7 +26157,7 @@
         </is>
       </c>
       <c r="E244" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F244" t="inlineStr">
         <is>
@@ -26893,7 +26893,7 @@
         </is>
       </c>
       <c r="E251" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F251" t="inlineStr">
         <is>
@@ -26997,7 +26997,7 @@
         </is>
       </c>
       <c r="E252" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F252" t="inlineStr">
         <is>
@@ -27521,7 +27521,7 @@
         </is>
       </c>
       <c r="E257" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F257" t="inlineStr">
         <is>
@@ -27953,7 +27953,7 @@
         </is>
       </c>
       <c r="E261" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F261" t="inlineStr">
         <is>
@@ -28493,7 +28493,7 @@
         </is>
       </c>
       <c r="E266" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F266" t="inlineStr">
         <is>
@@ -28709,7 +28709,7 @@
         </is>
       </c>
       <c r="E268" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F268" t="inlineStr">
         <is>
@@ -28925,7 +28925,7 @@
         </is>
       </c>
       <c r="E270" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F270" t="inlineStr">
         <is>
@@ -29029,7 +29029,7 @@
         </is>
       </c>
       <c r="E271" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F271" t="inlineStr">
         <is>
@@ -30605,7 +30605,7 @@
         </is>
       </c>
       <c r="E286" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F286" t="inlineStr">
         <is>
@@ -39850,7 +39850,7 @@
         </is>
       </c>
       <c r="E374" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F374" t="inlineStr">
         <is>
@@ -40274,7 +40274,7 @@
         </is>
       </c>
       <c r="E378" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F378" t="inlineStr">
         <is>
@@ -40482,7 +40482,7 @@
         </is>
       </c>
       <c r="E380" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F380" t="inlineStr">
         <is>
@@ -41014,7 +41014,7 @@
         </is>
       </c>
       <c r="E385" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F385" t="inlineStr">
         <is>
@@ -41222,7 +41222,7 @@
         </is>
       </c>
       <c r="E387" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F387" t="inlineStr">
         <is>
@@ -41434,7 +41434,7 @@
         </is>
       </c>
       <c r="E389" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F389" t="inlineStr">
         <is>
@@ -42494,7 +42494,7 @@
         </is>
       </c>
       <c r="E399" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -43646,7 +43646,7 @@
         </is>
       </c>
       <c r="E410" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F410" t="inlineStr">
         <is>
@@ -44590,7 +44590,7 @@
         </is>
       </c>
       <c r="E419" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F419" t="inlineStr">
         <is>
@@ -44694,7 +44694,7 @@
         </is>
       </c>
       <c r="E420" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F420" t="inlineStr">
         <is>
@@ -45002,7 +45002,7 @@
         </is>
       </c>
       <c r="E423" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F423" t="inlineStr">
         <is>
@@ -45210,7 +45210,7 @@
         </is>
       </c>
       <c r="E425" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F425" t="inlineStr">
         <is>
@@ -46159,7 +46159,7 @@
         </is>
       </c>
       <c r="E434" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F434" t="inlineStr">
         <is>
@@ -48169,7 +48169,7 @@
         </is>
       </c>
       <c r="E453" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F453" t="inlineStr">
         <is>
@@ -49233,7 +49233,7 @@
         </is>
       </c>
       <c r="E463" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F463" t="inlineStr">
         <is>
@@ -50181,7 +50181,7 @@
         </is>
       </c>
       <c r="E472" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F472" t="inlineStr">
         <is>
@@ -51017,7 +51017,7 @@
         </is>
       </c>
       <c r="E480" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F480" t="inlineStr">
         <is>
@@ -51121,7 +51121,7 @@
         </is>
       </c>
       <c r="E481" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F481" t="inlineStr">
         <is>
@@ -51225,7 +51225,7 @@
         </is>
       </c>
       <c r="E482" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F482" t="inlineStr">
         <is>
@@ -53001,7 +53001,7 @@
         </is>
       </c>
       <c r="E499" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F499" t="inlineStr">
         <is>

</xml_diff>